<commit_message>
prod and dev folders. Add PNG ods.
</commit_message>
<xml_diff>
--- a/data/2024M04_emp_info_raw.xlsx
+++ b/data/2024M04_emp_info_raw.xlsx
@@ -16,7 +16,7 @@
     <definedName name="empinfo">'empinfo'!$A$1:$R$310</definedName>
     <definedName name="salary">'salary'!$A$1:$E$320</definedName>
     <definedName name="jobcodes">'jobcodes'!$A$1:$C$235</definedName>
-    <definedName name="leave">'leave'!$A$1:$G$14</definedName>
+    <definedName name="leave">'leave'!$A$1:$F$14</definedName>
   </definedNames>
   <calcPr fullCalcOnLoad="true"/>
 </workbook>
@@ -31295,7 +31295,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1048576"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -31309,10 +31309,9 @@
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="41" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2131</v>
       </c>
@@ -31331,11 +31330,8 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2136</v>
       </c>
@@ -31354,11 +31350,8 @@
       <c r="F2">
         <v>63303356</v>
       </c>
-      <c r="G2" t="s">
-        <v>1249</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2136</v>
       </c>
@@ -31377,11 +31370,8 @@
       <c r="F3">
         <v>111111111</v>
       </c>
-      <c r="G3" t="s">
-        <v>1657</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2138</v>
       </c>
@@ -31400,11 +31390,8 @@
       <c r="F4">
         <v>111887176</v>
       </c>
-      <c r="G4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2140</v>
       </c>
@@ -31423,11 +31410,8 @@
       <c r="F5">
         <v>214011720</v>
       </c>
-      <c r="G5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2136</v>
       </c>
@@ -31446,11 +31430,8 @@
       <c r="F6">
         <v>333153667</v>
       </c>
-      <c r="G6" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2142</v>
       </c>
@@ -31469,11 +31450,8 @@
       <c r="F7">
         <v>333881903</v>
       </c>
-      <c r="G7" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2140</v>
       </c>
@@ -31492,11 +31470,8 @@
       <c r="F8">
         <v>333887115</v>
       </c>
-      <c r="G8" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2140</v>
       </c>
@@ -31515,11 +31490,8 @@
       <c r="F9">
         <v>333887315</v>
       </c>
-      <c r="G9" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2142</v>
       </c>
@@ -31538,11 +31510,8 @@
       <c r="F10">
         <v>333887700</v>
       </c>
-      <c r="G10" t="s">
-        <v>1466</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2138</v>
       </c>
@@ -31561,11 +31530,8 @@
       <c r="F11">
         <v>531886044</v>
       </c>
-      <c r="G11" t="s">
-        <v>974</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2138</v>
       </c>
@@ -31584,11 +31550,8 @@
       <c r="F12">
         <v>536639980</v>
       </c>
-      <c r="G12" t="s">
-        <v>1503</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2140</v>
       </c>
@@ -31607,11 +31570,8 @@
       <c r="F13">
         <v>709578766</v>
       </c>
-      <c r="G13" t="s">
-        <v>1060</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2142</v>
       </c>
@@ -31629,9 +31589,6 @@
       </c>
       <c r="F14">
         <v>730686313</v>
-      </c>
-      <c r="G14" t="s">
-        <v>990</v>
       </c>
     </row>
   </sheetData>

</xml_diff>